<commit_message>
stable version, added support for not found
</commit_message>
<xml_diff>
--- a/JUEGOS.xlsx
+++ b/JUEGOS.xlsx
@@ -1926,10 +1926,10 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.25"/>
@@ -3417,13 +3417,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.13"/>
   </cols>
@@ -4066,9 +4066,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>